<commit_message>
feat: initial rewrite of model
</commit_message>
<xml_diff>
--- a/files/imdhub-staging.xlsx
+++ b/files/imdhub-staging.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-rd-recon41md/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06721414-8F4B-E24B-919A-C43358ED4055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="740" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="79">
   <si>
     <t>tableName</t>
   </si>
@@ -28,6 +22,9 @@
     <t>columnName</t>
   </si>
   <si>
+    <t>label</t>
+  </si>
+  <si>
     <t>description</t>
   </si>
   <si>
@@ -37,13 +34,16 @@
     <t>key</t>
   </si>
   <si>
+    <t>semantics</t>
+  </si>
+  <si>
     <t>refSchema</t>
   </si>
   <si>
     <t>refTable</t>
   </si>
   <si>
-    <t>semantics</t>
+    <t>validation</t>
   </si>
   <si>
     <t>shouldImport</t>
@@ -52,19 +52,40 @@
     <t>Core clinical data</t>
   </si>
   <si>
-    <t>name of data source</t>
-  </si>
-  <si>
-    <t>participant identifier</t>
+    <t>date record was submitted</t>
+  </si>
+  <si>
+    <t>name of data provider</t>
+  </si>
+  <si>
+    <t>participant id</t>
   </si>
   <si>
     <t>center id</t>
   </si>
   <si>
-    <t>date record created</t>
-  </si>
-  <si>
-    <t>date record last modified</t>
+    <t>date record was created</t>
+  </si>
+  <si>
+    <t>date record was last modified</t>
+  </si>
+  <si>
+    <t>has given informed consent</t>
+  </si>
+  <si>
+    <t>date informed consent was given</t>
+  </si>
+  <si>
+    <t>has agreed to recontact of incidental findings</t>
+  </si>
+  <si>
+    <t>has agreed to future reuse</t>
+  </si>
+  <si>
+    <t>has agreed to recontact for future research</t>
+  </si>
+  <si>
+    <t>has agreed to shared family tree</t>
   </si>
   <si>
     <t>month of birth</t>
@@ -76,19 +97,85 @@
     <t>gender at birth</t>
   </si>
   <si>
-    <t>country of residence</t>
+    <t>country of residence of participant</t>
+  </si>
+  <si>
+    <t>country of residence of father</t>
+  </si>
+  <si>
+    <t>country of residence of mother</t>
   </si>
   <si>
     <t>Harmonised participant clinical metadata</t>
   </si>
   <si>
+    <t>Incidental findings of subject</t>
+  </si>
+  <si>
+    <t>Consent for shared family tree</t>
+  </si>
+  <si>
+    <t>Harmonised metadata submitted by the data provider</t>
+  </si>
+  <si>
+    <t>date the record (participant) was submitted by the data provider</t>
+  </si>
+  <si>
+    <t>name of the data provider as defined by the IMDHub providers list</t>
+  </si>
+  <si>
+    <t>the identifier that is used within the data provider's system</t>
+  </si>
+  <si>
+    <t>an identifier that links the participant to an organisation</t>
+  </si>
+  <si>
+    <t>date the record was created within the data provider's system</t>
+  </si>
+  <si>
+    <t>date the record was last modified within the data provider's system</t>
+  </si>
+  <si>
+    <t>an indication that the participant have consent within the data provider's system</t>
+  </si>
+  <si>
+    <t>the date informed consent was given</t>
+  </si>
+  <si>
+    <t>indication that the participant has agreed that their data can be reused in the future</t>
+  </si>
+  <si>
+    <t>indication that the participant has agreed that they can be contacted for future research</t>
+  </si>
+  <si>
+    <t>indication that the participant has agreed to sharing their family tree</t>
+  </si>
+  <si>
+    <t>the month the participant was born</t>
+  </si>
+  <si>
+    <t>the year the participant was born</t>
+  </si>
+  <si>
+    <t>ISO country name that indicates the current residence of the participant</t>
+  </si>
+  <si>
+    <t>ISO country name that indicates the current residence of the participant's father</t>
+  </si>
+  <si>
+    <t>ISO country name that indicates the current residence of the participant's mother</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
     <t>ontology</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
-    <t>date</t>
+    <t>bool</t>
   </si>
   <si>
     <t>int</t>
@@ -97,6 +184,51 @@
     <t>1</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164590</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25426</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0003071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93874</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C69199</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C114550</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93579</t>
+  </si>
+  <si>
+    <t>http://snomed.info/id/119297000</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000178</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000305</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000009</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83090</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GSSO_009418</t>
+  </si>
+  <si>
+    <t>http://snomed.info/id/416647007</t>
+  </si>
+  <si>
     <t>IMDHub Refs</t>
   </si>
   <si>
@@ -115,31 +247,15 @@
     <t>Countries</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25426</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0003071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93874</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C69199</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C114550</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83090</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GSSO_009418</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C177579</t>
+    <t>(function(){
+ const current_year = new Date().toLocaleDateString("en",{year: "numeric"});
+ if (yearOfBirth &lt; 1900) {
+  return 'Year of birth must be after the year 1900';
+ }
+ if (yearOfBirth &gt; current_year) {
+  return 'Year of birth cannot be greater than the current year';
+ }
+})();</t>
   </si>
   <si>
     <t>TRUE</t>
@@ -148,8 +264,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,21 +315,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -251,7 +359,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -285,7 +393,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -320,10 +427,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -496,16 +602,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,215 +637,451 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" t="s">
+        <v>71</v>
+      </c>
+      <c r="I18" t="s">
+        <v>76</v>
+      </c>
+      <c r="K18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I19" t="s">
+        <v>76</v>
+      </c>
+      <c r="K19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" t="s">
-        <v>40</v>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H20" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" t="s">
+        <v>76</v>
+      </c>
+      <c r="K20" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="H6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G3" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId2"/>
+    <hyperlink ref="G5" r:id="rId3"/>
+    <hyperlink ref="G6" r:id="rId4"/>
+    <hyperlink ref="G7" r:id="rId5"/>
+    <hyperlink ref="G8" r:id="rId6"/>
+    <hyperlink ref="G9" r:id="rId7"/>
+    <hyperlink ref="G10" r:id="rId8"/>
+    <hyperlink ref="G11" r:id="rId9"/>
+    <hyperlink ref="G12" r:id="rId10"/>
+    <hyperlink ref="G13" r:id="rId11"/>
+    <hyperlink ref="G15" r:id="rId12"/>
+    <hyperlink ref="G16" r:id="rId13"/>
+    <hyperlink ref="G17" r:id="rId14"/>
+    <hyperlink ref="G18" r:id="rId15"/>
+    <hyperlink ref="G19" r:id="rId16"/>
+    <hyperlink ref="G20" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: added expressions for staging table
</commit_message>
<xml_diff>
--- a/files/imdhub-staging.xlsx
+++ b/files/imdhub-staging.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="82">
   <si>
     <t>tableName</t>
   </si>
@@ -245,6 +245,60 @@
   </si>
   <si>
     <t>Countries</t>
+  </si>
+  <si>
+    <t>(function() {
+  if (dateRecordWasCreated !== null) {
+    const today = new Date();
+    const earliestDate = new Date("2015-01-01");
+    const input = new Date(dateRecordWasCreated);
+    const todayParsed = Date.parse(today);
+    const inputParsed = Date.parse(input);
+    const earliestParsed = Date.parse(earliestDate);
+    if (inputParsed &lt; earliestParsed) {
+      return "The date the record was created cannot be earlier than 01 January 2015";
+    }
+    if (inputParsed &gt; todayParsed) {
+      return "The date the record was created cannot be greater than today";
+    }
+  }
+})();</t>
+  </si>
+  <si>
+    <t>(function() {
+  if (dateRecordWasLastModified !== null) {
+    const today = new Date();
+    const earliestDate = new Date("2015-01-01");
+    const input = new Date(dateRecordWasLastModified);
+    const todayParsed = Date.parse(today);
+    const inputParsed = Date.parse(input);
+    const earliestParsed = Date.parse(earliestDate);
+    if (inputParsed &lt; earliestParsed) {
+      return "The date the record was created cannot be earlier than 01 January 2015";
+    }
+    if (inputParsed &gt; todayParsed) {
+      return "The date the record was created cannot be greater than today";
+    }
+  }
+})();</t>
+  </si>
+  <si>
+    <t>(function() {
+  if (dateInformedConsentWasGiven !== null) {
+    const today = new Date();
+    const earliestDate = new Date("2015-01-01");
+    const input = new Date(dateInformedConsentWasGiven);
+    const todayParsed = Date.parse(today);
+    const inputParsed = Date.parse(input);
+    const earliestParsed = Date.parse(earliestDate);
+    if (inputParsed &lt; earliestParsed) {
+      return "The date the record was created cannot be earlier than 01 January 2015";
+    }
+    if (inputParsed &gt; todayParsed) {
+      return "The date the record was created cannot be greater than today";
+    }
+  }
+})();</t>
   </si>
   <si>
     <t>(function(){
@@ -655,7 +709,7 @@
         <v>33</v>
       </c>
       <c r="K2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -675,7 +729,7 @@
         <v>56</v>
       </c>
       <c r="K3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -701,7 +755,7 @@
         <v>72</v>
       </c>
       <c r="K4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -724,7 +778,7 @@
         <v>58</v>
       </c>
       <c r="K5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -750,7 +804,7 @@
         <v>73</v>
       </c>
       <c r="K6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -769,8 +823,11 @@
       <c r="G7" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="J7" t="s">
+        <v>77</v>
+      </c>
       <c r="K7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -789,8 +846,11 @@
       <c r="G8" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="J8" t="s">
+        <v>78</v>
+      </c>
       <c r="K8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -810,7 +870,7 @@
         <v>62</v>
       </c>
       <c r="K9" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -829,8 +889,11 @@
       <c r="G10" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="J10" t="s">
+        <v>79</v>
+      </c>
       <c r="K10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -850,7 +913,7 @@
         <v>64</v>
       </c>
       <c r="K11" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -870,7 +933,7 @@
         <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -890,7 +953,7 @@
         <v>66</v>
       </c>
       <c r="K13" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -910,7 +973,7 @@
         <v>53</v>
       </c>
       <c r="K14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -936,7 +999,7 @@
         <v>74</v>
       </c>
       <c r="K15" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -956,10 +1019,10 @@
         <v>68</v>
       </c>
       <c r="J16" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="K16" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -982,7 +1045,7 @@
         <v>75</v>
       </c>
       <c r="K17" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1008,7 +1071,7 @@
         <v>76</v>
       </c>
       <c r="K18" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1034,7 +1097,7 @@
         <v>76</v>
       </c>
       <c r="K19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1060,7 +1123,7 @@
         <v>76</v>
       </c>
       <c r="K20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>